<commit_message>
aaaa api update on coursePromotion
</commit_message>
<xml_diff>
--- a/iShangkeProject/Design/API Permission Doc.xlsx
+++ b/iShangkeProject/Design/API Permission Doc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27300" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="11080" yWindow="0" windowWidth="27300" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="169">
   <si>
     <t xml:space="preserve">API Path </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -644,6 +644,50 @@
   </si>
   <si>
     <t>Query Course Comment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query Course Promotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create Course Promotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update Course Promotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Course Promotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/coursePromotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/coursePromotion/{id}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/coursePromotion/{id}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -708,7 +752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -794,12 +838,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,6 +876,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="好" xfId="1" builtinId="26"/>
@@ -1155,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -2263,18 +2320,18 @@
       <c r="C74" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="15"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="16"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="11"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="2" t="s">
@@ -2286,11 +2343,11 @@
       <c r="C76" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="4"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="12"/>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="2" t="s">
@@ -2334,18 +2391,18 @@
       <c r="C79" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="4"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="11"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="2" t="s">
@@ -2357,11 +2414,11 @@
       <c r="C81" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="4"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="12"/>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="2" t="s">
@@ -2405,18 +2462,18 @@
       <c r="C84" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="4"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="6"/>
     </row>
     <row r="85" spans="1:8">
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="11"/>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="2" t="s">
@@ -2428,18 +2485,18 @@
       <c r="C86" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="4"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="18"/>
     </row>
     <row r="87" spans="1:8">
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="11"/>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="2" t="s">
@@ -2451,11 +2508,11 @@
       <c r="C88" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="4"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="12"/>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" s="2" t="s">
@@ -2490,39 +2547,75 @@
       <c r="H90" s="4"/>
     </row>
     <row r="91" spans="1:8">
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="11"/>
     </row>
     <row r="92" spans="1:8">
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
+      <c r="A92" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
     </row>
     <row r="93" spans="1:8">
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
+      <c r="A93" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8">
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
+      <c r="A94" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:8">
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
+      <c r="A95" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
     </row>
     <row r="96" spans="1:8">
       <c r="D96" s="8"/>

</xml_diff>